<commit_message>
27-03_desired sliders work straight away without having to change discharging power
</commit_message>
<xml_diff>
--- a/Outputted Data.xlsx
+++ b/Outputted Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Outputted Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -447,10 +447,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -849,6 +849,550 @@
         <v>50000</v>
       </c>
     </row>
+    <row r="6">
+      <c r="B6" t="n">
+        <v>543.34176935416</v>
+      </c>
+      <c r="C6" t="n">
+        <v>35</v>
+      </c>
+      <c r="D6" t="n">
+        <v>289296</v>
+      </c>
+      <c r="E6" t="n">
+        <v>447.2035863348277</v>
+      </c>
+      <c r="F6" t="n">
+        <v>86788.8</v>
+      </c>
+      <c r="G6" t="n">
+        <v>72324</v>
+      </c>
+      <c r="H6" t="n">
+        <v>127</v>
+      </c>
+      <c r="I6" t="n">
+        <v>98</v>
+      </c>
+      <c r="J6" t="n">
+        <v>41</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1233</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P6" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R6" t="n">
+        <v>64000</v>
+      </c>
+      <c r="S6" t="n">
+        <v>450.8</v>
+      </c>
+      <c r="T6" t="n">
+        <v>412</v>
+      </c>
+      <c r="U6" t="n">
+        <v>245</v>
+      </c>
+      <c r="V6" t="n">
+        <v>170000</v>
+      </c>
+      <c r="W6" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="n">
+        <v>642.5622171730914</v>
+      </c>
+      <c r="C7" t="n">
+        <v>77</v>
+      </c>
+      <c r="D7" t="n">
+        <v>342216</v>
+      </c>
+      <c r="E7" t="n">
+        <v>447.9235806389746</v>
+      </c>
+      <c r="F7" t="n">
+        <v>78321.60000000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>85554.00000000001</v>
+      </c>
+      <c r="H7" t="n">
+        <v>111</v>
+      </c>
+      <c r="I7" t="n">
+        <v>49</v>
+      </c>
+      <c r="J7" t="n">
+        <v>30</v>
+      </c>
+      <c r="K7" t="n">
+        <v>127</v>
+      </c>
+      <c r="L7" t="n">
+        <v>49</v>
+      </c>
+      <c r="M7" t="n">
+        <v>28</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1233</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P7" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R7" t="n">
+        <v>64000</v>
+      </c>
+      <c r="S7" t="n">
+        <v>450.8</v>
+      </c>
+      <c r="T7" t="n">
+        <v>412</v>
+      </c>
+      <c r="U7" t="n">
+        <v>245</v>
+      </c>
+      <c r="V7" t="n">
+        <v>170000</v>
+      </c>
+      <c r="W7" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="n">
+        <v>495.5216781932683</v>
+      </c>
+      <c r="C8" t="n">
+        <v>63</v>
+      </c>
+      <c r="D8" t="n">
+        <v>347913.9</v>
+      </c>
+      <c r="E8" t="n">
+        <v>415.7809128630705</v>
+      </c>
+      <c r="F8" t="n">
+        <v>87149.5</v>
+      </c>
+      <c r="G8" t="n">
+        <v>65191.10000000001</v>
+      </c>
+      <c r="H8" t="n">
+        <v>112</v>
+      </c>
+      <c r="I8" t="n">
+        <v>49</v>
+      </c>
+      <c r="J8" t="n">
+        <v>5</v>
+      </c>
+      <c r="K8" t="n">
+        <v>39</v>
+      </c>
+      <c r="L8" t="n">
+        <v>47</v>
+      </c>
+      <c r="M8" t="n">
+        <v>4</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1233</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R8" t="n">
+        <v>64000</v>
+      </c>
+      <c r="S8" t="n">
+        <v>450.8</v>
+      </c>
+      <c r="T8" t="n">
+        <v>412</v>
+      </c>
+      <c r="U8" t="n">
+        <v>245</v>
+      </c>
+      <c r="V8" t="n">
+        <v>170000</v>
+      </c>
+      <c r="W8" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="n">
+        <v>545.4168935434984</v>
+      </c>
+      <c r="C9" t="n">
+        <v>63</v>
+      </c>
+      <c r="D9" t="n">
+        <v>599686.5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>441.1219917012447</v>
+      </c>
+      <c r="F9" t="n">
+        <v>96187</v>
+      </c>
+      <c r="G9" t="n">
+        <v>72436.70000000001</v>
+      </c>
+      <c r="H9" t="n">
+        <v>111</v>
+      </c>
+      <c r="I9" t="n">
+        <v>49</v>
+      </c>
+      <c r="J9" t="n">
+        <v>24</v>
+      </c>
+      <c r="K9" t="n">
+        <v>142</v>
+      </c>
+      <c r="L9" t="n">
+        <v>49</v>
+      </c>
+      <c r="M9" t="n">
+        <v>20</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1233</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P9" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R9" t="n">
+        <v>64000</v>
+      </c>
+      <c r="S9" t="n">
+        <v>450.8</v>
+      </c>
+      <c r="T9" t="n">
+        <v>412</v>
+      </c>
+      <c r="U9" t="n">
+        <v>245</v>
+      </c>
+      <c r="V9" t="n">
+        <v>170000</v>
+      </c>
+      <c r="W9" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="n">
+        <v>495.5216781932683</v>
+      </c>
+      <c r="C10" t="n">
+        <v>63</v>
+      </c>
+      <c r="D10" t="n">
+        <v>347913.9</v>
+      </c>
+      <c r="E10" t="n">
+        <v>415.7809128630705</v>
+      </c>
+      <c r="F10" t="n">
+        <v>87149.5</v>
+      </c>
+      <c r="G10" t="n">
+        <v>65191.10000000001</v>
+      </c>
+      <c r="H10" t="n">
+        <v>112</v>
+      </c>
+      <c r="I10" t="n">
+        <v>49</v>
+      </c>
+      <c r="J10" t="n">
+        <v>5</v>
+      </c>
+      <c r="K10" t="n">
+        <v>39</v>
+      </c>
+      <c r="L10" t="n">
+        <v>47</v>
+      </c>
+      <c r="M10" t="n">
+        <v>4</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1233</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P10" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R10" t="n">
+        <v>64000</v>
+      </c>
+      <c r="S10" t="n">
+        <v>450.8</v>
+      </c>
+      <c r="T10" t="n">
+        <v>412</v>
+      </c>
+      <c r="U10" t="n">
+        <v>245</v>
+      </c>
+      <c r="V10" t="n">
+        <v>170000</v>
+      </c>
+      <c r="W10" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="n">
+        <v>514.5199814358043</v>
+      </c>
+      <c r="C11" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>295132.8</v>
+      </c>
+      <c r="E11" t="n">
+        <v>442.0016597510373</v>
+      </c>
+      <c r="F11" t="n">
+        <v>115485.6</v>
+      </c>
+      <c r="G11" t="n">
+        <v>68355.60000000002</v>
+      </c>
+      <c r="H11" t="n">
+        <v>111</v>
+      </c>
+      <c r="I11" t="n">
+        <v>50</v>
+      </c>
+      <c r="J11" t="n">
+        <v>25</v>
+      </c>
+      <c r="K11" t="n">
+        <v>96</v>
+      </c>
+      <c r="L11" t="n">
+        <v>48</v>
+      </c>
+      <c r="M11" t="n">
+        <v>17</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1233</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P11" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R11" t="n">
+        <v>45000</v>
+      </c>
+      <c r="S11" t="n">
+        <v>450.8</v>
+      </c>
+      <c r="T11" t="n">
+        <v>412</v>
+      </c>
+      <c r="U11" t="n">
+        <v>245</v>
+      </c>
+      <c r="V11" t="n">
+        <v>170000</v>
+      </c>
+      <c r="W11" t="n">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="n">
+        <v>746.3673234890744</v>
+      </c>
+      <c r="C12" t="n">
+        <v>126</v>
+      </c>
+      <c r="D12" t="n">
+        <v>260632.08</v>
+      </c>
+      <c r="E12" t="n">
+        <v>449.5668049792531</v>
+      </c>
+      <c r="F12" t="n">
+        <v>72841.68000000001</v>
+      </c>
+      <c r="G12" t="n">
+        <v>99435.60000000001</v>
+      </c>
+      <c r="H12" t="n">
+        <v>111</v>
+      </c>
+      <c r="I12" t="n">
+        <v>42</v>
+      </c>
+      <c r="J12" t="n">
+        <v>27</v>
+      </c>
+      <c r="K12" t="n">
+        <v>320</v>
+      </c>
+      <c r="L12" t="n">
+        <v>54</v>
+      </c>
+      <c r="M12" t="n">
+        <v>75</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1233</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P12" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R12" t="n">
+        <v>90000</v>
+      </c>
+      <c r="S12" t="n">
+        <v>450.8</v>
+      </c>
+      <c r="T12" t="n">
+        <v>412</v>
+      </c>
+      <c r="U12" t="n">
+        <v>245</v>
+      </c>
+      <c r="V12" t="n">
+        <v>170000</v>
+      </c>
+      <c r="W12" t="n">
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="n">
+        <v>458.1427332831215</v>
+      </c>
+      <c r="C13" t="n">
+        <v>46.66666666666666</v>
+      </c>
+      <c r="D13" t="n">
+        <v>192384</v>
+      </c>
+      <c r="E13" t="n">
+        <v>446.442410462481</v>
+      </c>
+      <c r="F13" t="n">
+        <v>141631.2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>60966</v>
+      </c>
+      <c r="H13" t="n">
+        <v>164</v>
+      </c>
+      <c r="I13" t="n">
+        <v>45</v>
+      </c>
+      <c r="J13" t="n">
+        <v>4</v>
+      </c>
+      <c r="K13" t="n">
+        <v>127</v>
+      </c>
+      <c r="L13" t="n">
+        <v>53</v>
+      </c>
+      <c r="M13" t="n">
+        <v>29</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1233</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P13" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R13" t="n">
+        <v>50000</v>
+      </c>
+      <c r="S13" t="n">
+        <v>450.8</v>
+      </c>
+      <c r="T13" t="n">
+        <v>412</v>
+      </c>
+      <c r="U13" t="n">
+        <v>245</v>
+      </c>
+      <c r="V13" t="n">
+        <v>170000</v>
+      </c>
+      <c r="W13" t="n">
+        <v>120000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
29-03_change min charging time to km/min
</commit_message>
<xml_diff>
--- a/Outputted Data.xlsx
+++ b/Outputted Data.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X13"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
@@ -1393,6 +1393,754 @@
         <v>120000</v>
       </c>
     </row>
+    <row r="14">
+      <c r="B14" t="n">
+        <v>636.4307446591522</v>
+      </c>
+      <c r="C14" t="n">
+        <v>84</v>
+      </c>
+      <c r="D14" t="n">
+        <v>304326</v>
+      </c>
+      <c r="E14" t="n">
+        <v>441.7270867956914</v>
+      </c>
+      <c r="F14" t="n">
+        <v>77459.76000000001</v>
+      </c>
+      <c r="G14" t="n">
+        <v>86402.16</v>
+      </c>
+      <c r="H14" t="n">
+        <v>111</v>
+      </c>
+      <c r="I14" t="n">
+        <v>54</v>
+      </c>
+      <c r="J14" t="n">
+        <v>26</v>
+      </c>
+      <c r="K14" t="n">
+        <v>165</v>
+      </c>
+      <c r="L14" t="n">
+        <v>53</v>
+      </c>
+      <c r="M14" t="n">
+        <v>26</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1305</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P14" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R14" t="n">
+        <v>64800</v>
+      </c>
+      <c r="S14" t="n">
+        <v>442</v>
+      </c>
+      <c r="T14" t="n">
+        <v>450</v>
+      </c>
+      <c r="U14" t="n">
+        <v>245</v>
+      </c>
+      <c r="V14" t="n">
+        <v>150000</v>
+      </c>
+      <c r="W14" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="n">
+        <v>520.9892660409712</v>
+      </c>
+      <c r="C15" t="n">
+        <v>35</v>
+      </c>
+      <c r="D15" t="n">
+        <v>282384</v>
+      </c>
+      <c r="E15" t="n">
+        <v>436.5187818828257</v>
+      </c>
+      <c r="F15" t="n">
+        <v>84715.20000000001</v>
+      </c>
+      <c r="G15" t="n">
+        <v>70596</v>
+      </c>
+      <c r="H15" t="n">
+        <v>127</v>
+      </c>
+      <c r="I15" t="n">
+        <v>106</v>
+      </c>
+      <c r="J15" t="n">
+        <v>37</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1305</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P15" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R15" t="n">
+        <v>64800</v>
+      </c>
+      <c r="S15" t="n">
+        <v>442</v>
+      </c>
+      <c r="T15" t="n">
+        <v>450</v>
+      </c>
+      <c r="U15" t="n">
+        <v>245</v>
+      </c>
+      <c r="V15" t="n">
+        <v>150000</v>
+      </c>
+      <c r="W15" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="n">
+        <v>529.9095920387473</v>
+      </c>
+      <c r="C16" t="n">
+        <v>63</v>
+      </c>
+      <c r="D16" t="n">
+        <v>594708.3</v>
+      </c>
+      <c r="E16" t="n">
+        <v>437.4406639004148</v>
+      </c>
+      <c r="F16" t="n">
+        <v>95385.24000000001</v>
+      </c>
+      <c r="G16" t="n">
+        <v>71828.82000000001</v>
+      </c>
+      <c r="H16" t="n">
+        <v>111</v>
+      </c>
+      <c r="I16" t="n">
+        <v>53</v>
+      </c>
+      <c r="J16" t="n">
+        <v>22</v>
+      </c>
+      <c r="K16" t="n">
+        <v>142</v>
+      </c>
+      <c r="L16" t="n">
+        <v>54</v>
+      </c>
+      <c r="M16" t="n">
+        <v>18</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1305</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P16" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R16" t="n">
+        <v>64800</v>
+      </c>
+      <c r="S16" t="n">
+        <v>442</v>
+      </c>
+      <c r="T16" t="n">
+        <v>450</v>
+      </c>
+      <c r="U16" t="n">
+        <v>245</v>
+      </c>
+      <c r="V16" t="n">
+        <v>150000</v>
+      </c>
+      <c r="W16" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="n">
+        <v>584.8320029033736</v>
+      </c>
+      <c r="C17" t="n">
+        <v>42.00000000000001</v>
+      </c>
+      <c r="D17" t="n">
+        <v>337824</v>
+      </c>
+      <c r="E17" t="n">
+        <v>375.9535269709544</v>
+      </c>
+      <c r="F17" t="n">
+        <v>77500.80000000002</v>
+      </c>
+      <c r="G17" t="n">
+        <v>77500.8</v>
+      </c>
+      <c r="H17" t="n">
+        <v>111</v>
+      </c>
+      <c r="I17" t="n">
+        <v>104</v>
+      </c>
+      <c r="J17" t="n">
+        <v>18</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>1305</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P17" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R17" t="n">
+        <v>64800</v>
+      </c>
+      <c r="S17" t="n">
+        <v>442</v>
+      </c>
+      <c r="T17" t="n">
+        <v>450</v>
+      </c>
+      <c r="U17" t="n">
+        <v>245</v>
+      </c>
+      <c r="V17" t="n">
+        <v>150000</v>
+      </c>
+      <c r="W17" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="n">
+        <v>584.8320029033736</v>
+      </c>
+      <c r="C18" t="n">
+        <v>42.00000000000001</v>
+      </c>
+      <c r="D18" t="n">
+        <v>337824</v>
+      </c>
+      <c r="E18" t="n">
+        <v>375.9535269709544</v>
+      </c>
+      <c r="F18" t="n">
+        <v>77500.80000000002</v>
+      </c>
+      <c r="G18" t="n">
+        <v>77500.8</v>
+      </c>
+      <c r="H18" t="n">
+        <v>111</v>
+      </c>
+      <c r="I18" t="n">
+        <v>104</v>
+      </c>
+      <c r="J18" t="n">
+        <v>18</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1305</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P18" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R18" t="n">
+        <v>64800</v>
+      </c>
+      <c r="S18" t="n">
+        <v>442</v>
+      </c>
+      <c r="T18" t="n">
+        <v>450</v>
+      </c>
+      <c r="U18" t="n">
+        <v>245</v>
+      </c>
+      <c r="V18" t="n">
+        <v>150000</v>
+      </c>
+      <c r="W18" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="n">
+        <v>526.9023976019301</v>
+      </c>
+      <c r="C19" t="n">
+        <v>60.66666666666667</v>
+      </c>
+      <c r="D19" t="n">
+        <v>315108</v>
+      </c>
+      <c r="E19" t="n">
+        <v>441.1797804915752</v>
+      </c>
+      <c r="F19" t="n">
+        <v>93046.32000000001</v>
+      </c>
+      <c r="G19" t="n">
+        <v>71518.32000000001</v>
+      </c>
+      <c r="H19" t="n">
+        <v>165</v>
+      </c>
+      <c r="I19" t="n">
+        <v>54</v>
+      </c>
+      <c r="J19" t="n">
+        <v>49</v>
+      </c>
+      <c r="K19" t="n">
+        <v>326</v>
+      </c>
+      <c r="L19" t="n">
+        <v>52</v>
+      </c>
+      <c r="M19" t="n">
+        <v>23</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1305</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P19" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R19" t="n">
+        <v>64800</v>
+      </c>
+      <c r="S19" t="n">
+        <v>442</v>
+      </c>
+      <c r="T19" t="n">
+        <v>450</v>
+      </c>
+      <c r="U19" t="n">
+        <v>245</v>
+      </c>
+      <c r="V19" t="n">
+        <v>150000</v>
+      </c>
+      <c r="W19" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="n">
+        <v>575.4045678431019</v>
+      </c>
+      <c r="C20" t="n">
+        <v>71.40000000000001</v>
+      </c>
+      <c r="D20" t="n">
+        <v>398048.4</v>
+      </c>
+      <c r="E20" t="n">
+        <v>436.596427135095</v>
+      </c>
+      <c r="F20" t="n">
+        <v>84430.80000000002</v>
+      </c>
+      <c r="G20" t="n">
+        <v>77971.68000000001</v>
+      </c>
+      <c r="H20" t="n">
+        <v>111</v>
+      </c>
+      <c r="I20" t="n">
+        <v>53</v>
+      </c>
+      <c r="J20" t="n">
+        <v>24</v>
+      </c>
+      <c r="K20" t="n">
+        <v>126</v>
+      </c>
+      <c r="L20" t="n">
+        <v>54</v>
+      </c>
+      <c r="M20" t="n">
+        <v>31</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1305</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P20" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R20" t="n">
+        <v>64800</v>
+      </c>
+      <c r="S20" t="n">
+        <v>442</v>
+      </c>
+      <c r="T20" t="n">
+        <v>450</v>
+      </c>
+      <c r="U20" t="n">
+        <v>245</v>
+      </c>
+      <c r="V20" t="n">
+        <v>150000</v>
+      </c>
+      <c r="W20" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="n">
+        <v>666.7622210379019</v>
+      </c>
+      <c r="C21" t="n">
+        <v>42.00000000000001</v>
+      </c>
+      <c r="D21" t="n">
+        <v>452088</v>
+      </c>
+      <c r="E21" t="n">
+        <v>438.6124481327801</v>
+      </c>
+      <c r="F21" t="n">
+        <v>90417.60000000001</v>
+      </c>
+      <c r="G21" t="n">
+        <v>90417.60000000001</v>
+      </c>
+      <c r="H21" t="n">
+        <v>111</v>
+      </c>
+      <c r="I21" t="n">
+        <v>104</v>
+      </c>
+      <c r="J21" t="n">
+        <v>21</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1305</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P21" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R21" t="n">
+        <v>90000</v>
+      </c>
+      <c r="S21" t="n">
+        <v>442</v>
+      </c>
+      <c r="T21" t="n">
+        <v>450</v>
+      </c>
+      <c r="U21" t="n">
+        <v>245</v>
+      </c>
+      <c r="V21" t="n">
+        <v>150000</v>
+      </c>
+      <c r="W21" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="n">
+        <v>634.6512220340331</v>
+      </c>
+      <c r="C22" t="n">
+        <v>42</v>
+      </c>
+      <c r="D22" t="n">
+        <v>426420</v>
+      </c>
+      <c r="E22" t="n">
+        <v>413.7095435684647</v>
+      </c>
+      <c r="F22" t="n">
+        <v>85284.00000000001</v>
+      </c>
+      <c r="G22" t="n">
+        <v>85284.00000000001</v>
+      </c>
+      <c r="H22" t="n">
+        <v>111</v>
+      </c>
+      <c r="I22" t="n">
+        <v>103</v>
+      </c>
+      <c r="J22" t="n">
+        <v>20</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1305</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P22" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R22" t="n">
+        <v>80000</v>
+      </c>
+      <c r="S22" t="n">
+        <v>442</v>
+      </c>
+      <c r="T22" t="n">
+        <v>450</v>
+      </c>
+      <c r="U22" t="n">
+        <v>245</v>
+      </c>
+      <c r="V22" t="n">
+        <v>150000</v>
+      </c>
+      <c r="W22" t="n">
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="n">
+        <v>477.1847142868455</v>
+      </c>
+      <c r="C23" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="D23" t="n">
+        <v>263979</v>
+      </c>
+      <c r="E23" t="n">
+        <v>428.2157676348548</v>
+      </c>
+      <c r="F23" t="n">
+        <v>142335.8</v>
+      </c>
+      <c r="G23" t="n">
+        <v>64465</v>
+      </c>
+      <c r="H23" t="n">
+        <v>112</v>
+      </c>
+      <c r="I23" t="n">
+        <v>50</v>
+      </c>
+      <c r="J23" t="n">
+        <v>5</v>
+      </c>
+      <c r="K23" t="n">
+        <v>163</v>
+      </c>
+      <c r="L23" t="n">
+        <v>55</v>
+      </c>
+      <c r="M23" t="n">
+        <v>4</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1305</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P23" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R23" t="n">
+        <v>60000</v>
+      </c>
+      <c r="S23" t="n">
+        <v>442</v>
+      </c>
+      <c r="T23" t="n">
+        <v>450</v>
+      </c>
+      <c r="U23" t="n">
+        <v>245</v>
+      </c>
+      <c r="V23" t="n">
+        <v>150000</v>
+      </c>
+      <c r="W23" t="n">
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="n">
+        <v>550.0116564627</v>
+      </c>
+      <c r="C24" t="n">
+        <v>63</v>
+      </c>
+      <c r="D24" t="n">
+        <v>583448.175</v>
+      </c>
+      <c r="E24" t="n">
+        <v>441.5900414937759</v>
+      </c>
+      <c r="F24" t="n">
+        <v>95677.89000000001</v>
+      </c>
+      <c r="G24" t="n">
+        <v>74666.145</v>
+      </c>
+      <c r="H24" t="n">
+        <v>111</v>
+      </c>
+      <c r="I24" t="n">
+        <v>54</v>
+      </c>
+      <c r="J24" t="n">
+        <v>24</v>
+      </c>
+      <c r="K24" t="n">
+        <v>142</v>
+      </c>
+      <c r="L24" t="n">
+        <v>51</v>
+      </c>
+      <c r="M24" t="n">
+        <v>17</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1305</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P24" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R24" t="n">
+        <v>70000</v>
+      </c>
+      <c r="S24" t="n">
+        <v>442</v>
+      </c>
+      <c r="T24" t="n">
+        <v>450</v>
+      </c>
+      <c r="U24" t="n">
+        <v>245</v>
+      </c>
+      <c r="V24" t="n">
+        <v>150000</v>
+      </c>
+      <c r="W24" t="n">
+        <v>95000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
01-04_Outputs BMS option to a new window
</commit_message>
<xml_diff>
--- a/Outputted Data.xlsx
+++ b/Outputted Data.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
@@ -2141,6 +2141,74 @@
         <v>95000</v>
       </c>
     </row>
+    <row r="25">
+      <c r="B25" t="n">
+        <v>543.34176935416</v>
+      </c>
+      <c r="C25" t="n">
+        <v>35</v>
+      </c>
+      <c r="D25" t="n">
+        <v>289296</v>
+      </c>
+      <c r="E25" t="n">
+        <v>447.2035863348277</v>
+      </c>
+      <c r="F25" t="n">
+        <v>86788.8</v>
+      </c>
+      <c r="G25" t="n">
+        <v>72324</v>
+      </c>
+      <c r="H25" t="n">
+        <v>127</v>
+      </c>
+      <c r="I25" t="n">
+        <v>98</v>
+      </c>
+      <c r="J25" t="n">
+        <v>41</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1233</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="P25" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R25" t="n">
+        <v>64000</v>
+      </c>
+      <c r="S25" t="n">
+        <v>450.8</v>
+      </c>
+      <c r="T25" t="n">
+        <v>412</v>
+      </c>
+      <c r="U25" t="n">
+        <v>245</v>
+      </c>
+      <c r="V25" t="n">
+        <v>170000</v>
+      </c>
+      <c r="W25" t="n">
+        <v>77000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
02-04_Fixed scatter plot crashing issue
</commit_message>
<xml_diff>
--- a/Outputted Data.xlsx
+++ b/Outputted Data.xlsx
@@ -447,10 +447,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X25"/>
+  <dimension ref="A1:X26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -2209,6 +2209,74 @@
         <v>77000</v>
       </c>
     </row>
+    <row r="26">
+      <c r="B26" t="n">
+        <v>451.5116343142244</v>
+      </c>
+      <c r="C26" t="n">
+        <v>84</v>
+      </c>
+      <c r="D26" t="n">
+        <v>90374.39999999999</v>
+      </c>
+      <c r="E26" t="n">
+        <v>306.8912637288979</v>
+      </c>
+      <c r="F26" t="n">
+        <v>50436</v>
+      </c>
+      <c r="G26" t="n">
+        <v>54129.6</v>
+      </c>
+      <c r="H26" t="n">
+        <v>135</v>
+      </c>
+      <c r="I26" t="n">
+        <v>35</v>
+      </c>
+      <c r="J26" t="n">
+        <v>2</v>
+      </c>
+      <c r="K26" t="n">
+        <v>165</v>
+      </c>
+      <c r="L26" t="n">
+        <v>60</v>
+      </c>
+      <c r="M26" t="n">
+        <v>28</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1171</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="P26" t="n">
+        <v>2.325</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="R26" t="n">
+        <v>28000</v>
+      </c>
+      <c r="S26" t="n">
+        <v>315</v>
+      </c>
+      <c r="T26" t="n">
+        <v>400</v>
+      </c>
+      <c r="U26" t="n">
+        <v>240</v>
+      </c>
+      <c r="V26" t="n">
+        <v>90000</v>
+      </c>
+      <c r="W26" t="n">
+        <v>50000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
03-04_Implemented increasing the req_energy to range
</commit_message>
<xml_diff>
--- a/Outputted Data.xlsx
+++ b/Outputted Data.xlsx
@@ -447,10 +447,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X26"/>
+  <dimension ref="A1:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="A26" sqref="A26:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -2211,69 +2211,853 @@
     </row>
     <row r="26">
       <c r="B26" t="n">
-        <v>451.5116343142244</v>
+        <v>213.4049414013323</v>
       </c>
       <c r="C26" t="n">
+        <v>11.144</v>
+      </c>
+      <c r="D26" t="n">
+        <v>13.40483300259625</v>
+      </c>
+      <c r="E26" t="n">
+        <v>231246</v>
+      </c>
+      <c r="F26" t="n">
+        <v>293.6298755186722</v>
+      </c>
+      <c r="G26" t="n">
+        <v>239880</v>
+      </c>
+      <c r="H26" t="n">
+        <v>28747.96</v>
+      </c>
+      <c r="I26" t="n">
+        <v>163</v>
+      </c>
+      <c r="J26" t="n">
+        <v>52</v>
+      </c>
+      <c r="K26" t="n">
+        <v>4</v>
+      </c>
+      <c r="L26" t="n">
+        <v>40</v>
+      </c>
+      <c r="M26" t="n">
+        <v>49</v>
+      </c>
+      <c r="N26" t="n">
+        <v>3</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1485</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>2.325</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S26" t="n">
+        <v>28000</v>
+      </c>
+      <c r="T26" t="n">
+        <v>315</v>
+      </c>
+      <c r="U26" t="n">
+        <v>400</v>
+      </c>
+      <c r="V26" t="n">
+        <v>240</v>
+      </c>
+      <c r="W26" t="n">
+        <v>90000</v>
+      </c>
+      <c r="X26" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="n">
+        <v>484.323441769288</v>
+      </c>
+      <c r="C27" t="n">
         <v>84</v>
       </c>
-      <c r="D26" t="n">
-        <v>90374.39999999999</v>
-      </c>
-      <c r="E26" t="n">
-        <v>306.8912637288979</v>
-      </c>
-      <c r="F26" t="n">
-        <v>50436</v>
-      </c>
-      <c r="G26" t="n">
-        <v>54129.6</v>
-      </c>
-      <c r="H26" t="n">
-        <v>135</v>
-      </c>
-      <c r="I26" t="n">
-        <v>35</v>
-      </c>
-      <c r="J26" t="n">
-        <v>2</v>
-      </c>
-      <c r="K26" t="n">
+      <c r="D27" t="n">
+        <v>4.036028681410734</v>
+      </c>
+      <c r="E27" t="n">
+        <v>120600</v>
+      </c>
+      <c r="F27" t="n">
+        <v>306.5161307454832</v>
+      </c>
+      <c r="G27" t="n">
+        <v>50320.08</v>
+      </c>
+      <c r="H27" t="n">
+        <v>58103.28</v>
+      </c>
+      <c r="I27" t="n">
+        <v>111</v>
+      </c>
+      <c r="J27" t="n">
+        <v>47</v>
+      </c>
+      <c r="K27" t="n">
+        <v>14</v>
+      </c>
+      <c r="L27" t="n">
         <v>165</v>
       </c>
-      <c r="L26" t="n">
-        <v>60</v>
-      </c>
-      <c r="M26" t="n">
+      <c r="M27" t="n">
+        <v>47</v>
+      </c>
+      <c r="N27" t="n">
+        <v>32</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1171</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S27" t="n">
+        <v>27700</v>
+      </c>
+      <c r="T27" t="n">
+        <v>315</v>
+      </c>
+      <c r="U27" t="n">
+        <v>398</v>
+      </c>
+      <c r="V27" t="n">
+        <v>240</v>
+      </c>
+      <c r="W27" t="n">
+        <v>90000</v>
+      </c>
+      <c r="X27" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="n">
+        <v>242.2955009345596</v>
+      </c>
+      <c r="C28" t="n">
+        <v>11.144</v>
+      </c>
+      <c r="D28" t="n">
+        <v>15.21956664161806</v>
+      </c>
+      <c r="E28" t="n">
+        <v>227682</v>
+      </c>
+      <c r="F28" t="n">
+        <v>294.4796680497925</v>
+      </c>
+      <c r="G28" t="n">
+        <v>236910</v>
+      </c>
+      <c r="H28" t="n">
+        <v>28923.92</v>
+      </c>
+      <c r="I28" t="n">
+        <v>163</v>
+      </c>
+      <c r="J28" t="n">
+        <v>53</v>
+      </c>
+      <c r="K28" t="n">
+        <v>4</v>
+      </c>
+      <c r="L28" t="n">
+        <v>40</v>
+      </c>
+      <c r="M28" t="n">
+        <v>48</v>
+      </c>
+      <c r="N28" t="n">
+        <v>3</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1171</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S28" t="n">
+        <v>27700</v>
+      </c>
+      <c r="T28" t="n">
+        <v>315</v>
+      </c>
+      <c r="U28" t="n">
+        <v>398</v>
+      </c>
+      <c r="V28" t="n">
+        <v>240</v>
+      </c>
+      <c r="W28" t="n">
+        <v>90000</v>
+      </c>
+      <c r="X28" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>277.1870672686526</v>
+      </c>
+      <c r="C29" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="D29" t="n">
+        <v>8.662095852145395</v>
+      </c>
+      <c r="E29" t="n">
+        <v>103635</v>
+      </c>
+      <c r="F29" t="n">
+        <v>306.9875518672199</v>
+      </c>
+      <c r="G29" t="n">
+        <v>122565</v>
+      </c>
+      <c r="H29" t="n">
+        <v>33260</v>
+      </c>
+      <c r="I29" t="n">
+        <v>163</v>
+      </c>
+      <c r="J29" t="n">
+        <v>56</v>
+      </c>
+      <c r="K29" t="n">
+        <v>4</v>
+      </c>
+      <c r="L29" t="n">
+        <v>53</v>
+      </c>
+      <c r="M29" t="n">
+        <v>38</v>
+      </c>
+      <c r="N29" t="n">
+        <v>4</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1171</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S29" t="n">
+        <v>27700</v>
+      </c>
+      <c r="T29" t="n">
+        <v>315</v>
+      </c>
+      <c r="U29" t="n">
+        <v>398</v>
+      </c>
+      <c r="V29" t="n">
+        <v>240</v>
+      </c>
+      <c r="W29" t="n">
+        <v>90000</v>
+      </c>
+      <c r="X29" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="n">
+        <v>484.323441769288</v>
+      </c>
+      <c r="C30" t="n">
+        <v>84</v>
+      </c>
+      <c r="D30" t="n">
+        <v>4.036028681410734</v>
+      </c>
+      <c r="E30" t="n">
+        <v>120600</v>
+      </c>
+      <c r="F30" t="n">
+        <v>306.5161307454832</v>
+      </c>
+      <c r="G30" t="n">
+        <v>50320.08</v>
+      </c>
+      <c r="H30" t="n">
+        <v>58103.28</v>
+      </c>
+      <c r="I30" t="n">
+        <v>111</v>
+      </c>
+      <c r="J30" t="n">
+        <v>47</v>
+      </c>
+      <c r="K30" t="n">
+        <v>14</v>
+      </c>
+      <c r="L30" t="n">
+        <v>165</v>
+      </c>
+      <c r="M30" t="n">
+        <v>47</v>
+      </c>
+      <c r="N30" t="n">
+        <v>32</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1171</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S30" t="n">
+        <v>27700</v>
+      </c>
+      <c r="T30" t="n">
+        <v>315</v>
+      </c>
+      <c r="U30" t="n">
+        <v>398</v>
+      </c>
+      <c r="V30" t="n">
+        <v>240</v>
+      </c>
+      <c r="W30" t="n">
+        <v>90000</v>
+      </c>
+      <c r="X30" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="n">
+        <v>500.8068765952128</v>
+      </c>
+      <c r="C31" t="n">
+        <v>84</v>
+      </c>
+      <c r="D31" t="n">
+        <v>4.173390638293441</v>
+      </c>
+      <c r="E31" t="n">
+        <v>180900</v>
+      </c>
+      <c r="F31" t="n">
+        <v>308.6595079373123</v>
+      </c>
+      <c r="G31" t="n">
+        <v>50404.68000000001</v>
+      </c>
+      <c r="H31" t="n">
+        <v>60133.68</v>
+      </c>
+      <c r="I31" t="n">
+        <v>111</v>
+      </c>
+      <c r="J31" t="n">
+        <v>47</v>
+      </c>
+      <c r="K31" t="n">
+        <v>20</v>
+      </c>
+      <c r="L31" t="n">
+        <v>165</v>
+      </c>
+      <c r="M31" t="n">
+        <v>47</v>
+      </c>
+      <c r="N31" t="n">
+        <v>22</v>
+      </c>
+      <c r="O31" t="n">
+        <v>1171</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S31" t="n">
+        <v>40000</v>
+      </c>
+      <c r="T31" t="n">
+        <v>315</v>
+      </c>
+      <c r="U31" t="n">
+        <v>398</v>
+      </c>
+      <c r="V31" t="n">
+        <v>240</v>
+      </c>
+      <c r="W31" t="n">
+        <v>90000</v>
+      </c>
+      <c r="X31" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>422.0531882892127</v>
+      </c>
+      <c r="C32" t="n">
+        <v>42</v>
+      </c>
+      <c r="D32" t="n">
+        <v>7.034219804820212</v>
+      </c>
+      <c r="E32" t="n">
+        <v>113022</v>
+      </c>
+      <c r="F32" t="n">
+        <v>283.35136806307</v>
+      </c>
+      <c r="G32" t="n">
+        <v>50150.88</v>
+      </c>
+      <c r="H32" t="n">
+        <v>50150.88</v>
+      </c>
+      <c r="I32" t="n">
+        <v>165</v>
+      </c>
+      <c r="J32" t="n">
+        <v>94</v>
+      </c>
+      <c r="K32" t="n">
+        <v>26</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1171</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S32" t="n">
+        <v>40000</v>
+      </c>
+      <c r="T32" t="n">
+        <v>315</v>
+      </c>
+      <c r="U32" t="n">
+        <v>398</v>
+      </c>
+      <c r="V32" t="n">
+        <v>240</v>
+      </c>
+      <c r="W32" t="n">
+        <v>90000</v>
+      </c>
+      <c r="X32" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>504.6793708753279</v>
+      </c>
+      <c r="C33" t="n">
+        <v>84</v>
+      </c>
+      <c r="D33" t="n">
+        <v>4.205661423961065</v>
+      </c>
+      <c r="E33" t="n">
+        <v>228528</v>
+      </c>
+      <c r="F33" t="n">
+        <v>309.0990589655484</v>
+      </c>
+      <c r="G33" t="n">
+        <v>54648</v>
+      </c>
+      <c r="H33" t="n">
+        <v>60609.60000000001</v>
+      </c>
+      <c r="I33" t="n">
+        <v>111</v>
+      </c>
+      <c r="J33" t="n">
+        <v>48</v>
+      </c>
+      <c r="K33" t="n">
+        <v>21</v>
+      </c>
+      <c r="L33" t="n">
+        <v>165</v>
+      </c>
+      <c r="M33" t="n">
+        <v>46</v>
+      </c>
+      <c r="N33" t="n">
+        <v>20</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1171</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S33" t="n">
+        <v>50000</v>
+      </c>
+      <c r="T33" t="n">
+        <v>315</v>
+      </c>
+      <c r="U33" t="n">
+        <v>398</v>
+      </c>
+      <c r="V33" t="n">
+        <v>240</v>
+      </c>
+      <c r="W33" t="n">
+        <v>90000</v>
+      </c>
+      <c r="X33" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>446.2492591759789</v>
+      </c>
+      <c r="C34" t="n">
+        <v>42</v>
+      </c>
+      <c r="D34" t="n">
+        <v>7.437487652932981</v>
+      </c>
+      <c r="E34" t="n">
+        <v>140616</v>
+      </c>
+      <c r="F34" t="n">
+        <v>301.9013757922399</v>
+      </c>
+      <c r="G34" t="n">
+        <v>53434.08</v>
+      </c>
+      <c r="H34" t="n">
+        <v>53434.07999999999</v>
+      </c>
+      <c r="I34" t="n">
+        <v>165</v>
+      </c>
+      <c r="J34" t="n">
+        <v>93</v>
+      </c>
+      <c r="K34" t="n">
         <v>28</v>
       </c>
-      <c r="N26" t="n">
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
         <v>1171</v>
       </c>
-      <c r="O26" t="n">
+      <c r="P34" t="n">
         <v>0.28</v>
       </c>
-      <c r="P26" t="n">
-        <v>2.325</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="R26" t="n">
-        <v>28000</v>
-      </c>
-      <c r="S26" t="n">
+      <c r="Q34" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S34" t="n">
+        <v>50000</v>
+      </c>
+      <c r="T34" t="n">
         <v>315</v>
       </c>
-      <c r="T26" t="n">
-        <v>400</v>
-      </c>
-      <c r="U26" t="n">
+      <c r="U34" t="n">
+        <v>398</v>
+      </c>
+      <c r="V34" t="n">
         <v>240</v>
       </c>
-      <c r="V26" t="n">
+      <c r="W34" t="n">
         <v>90000</v>
       </c>
-      <c r="W26" t="n">
+      <c r="X34" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="n">
+        <v>558.8017094888542</v>
+      </c>
+      <c r="C35" t="n">
+        <v>126</v>
+      </c>
+      <c r="D35" t="n">
+        <v>3.104453941604746</v>
+      </c>
+      <c r="E35" t="n">
+        <v>217721.52</v>
+      </c>
+      <c r="F35" t="n">
+        <v>309.2414937759336</v>
+      </c>
+      <c r="G35" t="n">
+        <v>53777.52</v>
+      </c>
+      <c r="H35" t="n">
+        <v>67113.36000000002</v>
+      </c>
+      <c r="I35" t="n">
+        <v>111</v>
+      </c>
+      <c r="J35" t="n">
+        <v>45</v>
+      </c>
+      <c r="K35" t="n">
+        <v>22</v>
+      </c>
+      <c r="L35" t="n">
+        <v>320</v>
+      </c>
+      <c r="M35" t="n">
+        <v>48</v>
+      </c>
+      <c r="N35" t="n">
+        <v>42</v>
+      </c>
+      <c r="O35" t="n">
+        <v>1171</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S35" t="n">
+        <v>60000</v>
+      </c>
+      <c r="T35" t="n">
+        <v>315</v>
+      </c>
+      <c r="U35" t="n">
+        <v>398</v>
+      </c>
+      <c r="V35" t="n">
+        <v>240</v>
+      </c>
+      <c r="W35" t="n">
+        <v>90000</v>
+      </c>
+      <c r="X35" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="n">
+        <v>420.0390040416348</v>
+      </c>
+      <c r="C36" t="n">
+        <v>50.40000000000001</v>
+      </c>
+      <c r="D36" t="n">
+        <v>5.833875056133818</v>
+      </c>
+      <c r="E36" t="n">
+        <v>171736</v>
+      </c>
+      <c r="F36" t="n">
+        <v>308.2107883817427</v>
+      </c>
+      <c r="G36" t="n">
+        <v>66866.5</v>
+      </c>
+      <c r="H36" t="n">
+        <v>50426.3</v>
+      </c>
+      <c r="I36" t="n">
+        <v>111</v>
+      </c>
+      <c r="J36" t="n">
+        <v>47</v>
+      </c>
+      <c r="K36" t="n">
+        <v>21</v>
+      </c>
+      <c r="L36" t="n">
+        <v>96</v>
+      </c>
+      <c r="M36" t="n">
+        <v>47</v>
+      </c>
+      <c r="N36" t="n">
+        <v>10</v>
+      </c>
+      <c r="O36" t="n">
+        <v>1171</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="R36" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S36" t="n">
+        <v>27700</v>
+      </c>
+      <c r="T36" t="n">
+        <v>315</v>
+      </c>
+      <c r="U36" t="n">
+        <v>398</v>
+      </c>
+      <c r="V36" t="n">
+        <v>240</v>
+      </c>
+      <c r="W36" t="n">
+        <v>90000</v>
+      </c>
+      <c r="X36" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="n">
+        <v>549.0243392415929</v>
+      </c>
+      <c r="C37" t="n">
+        <v>126</v>
+      </c>
+      <c r="D37" t="n">
+        <v>3.050135218008849</v>
+      </c>
+      <c r="E37" t="n">
+        <v>241544.16</v>
+      </c>
+      <c r="F37" t="n">
+        <v>309.0406639004149</v>
+      </c>
+      <c r="G37" t="n">
+        <v>54747.36000000001</v>
+      </c>
+      <c r="H37" t="n">
+        <v>65933.64000000001</v>
+      </c>
+      <c r="I37" t="n">
+        <v>111</v>
+      </c>
+      <c r="J37" t="n">
+        <v>47</v>
+      </c>
+      <c r="K37" t="n">
+        <v>25</v>
+      </c>
+      <c r="L37" t="n">
+        <v>320</v>
+      </c>
+      <c r="M37" t="n">
+        <v>46</v>
+      </c>
+      <c r="N37" t="n">
+        <v>29</v>
+      </c>
+      <c r="O37" t="n">
+        <v>1171</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="S37" t="n">
+        <v>40000</v>
+      </c>
+      <c r="T37" t="n">
+        <v>315</v>
+      </c>
+      <c r="U37" t="n">
+        <v>398</v>
+      </c>
+      <c r="V37" t="n">
+        <v>240</v>
+      </c>
+      <c r="W37" t="n">
+        <v>90000</v>
+      </c>
+      <c r="X37" t="n">
         <v>50000</v>
       </c>
     </row>

</xml_diff>